<commit_message>
updated pokemon_list.py to fix src image paths and not need variants variable.
</commit_message>
<xml_diff>
--- a/pokemon_list/data/pokemon_output.xlsx
+++ b/pokemon_list/data/pokemon_output.xlsx
@@ -4156,7 +4156,7 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/5/55/0350Milotic.png/70px-0350Milotic.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/3/34/0351Castform-Snowy.png/70px-0351Castform-Snowy.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/f/ff/0351Castform.png/70px-0351Castform.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/b/b6/0352Kecleon.png/70px-0352Kecleon.png</t>
@@ -4261,7 +4261,7 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/6/61/0385Jirachi.png/70px-0385Jirachi.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/1/17/0386Deoxys-Speed.png/70px-0386Deoxys-Speed.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/d/d7/0386Deoxys.png/70px-0386Deoxys.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/6/68/0387Turtwig.png/70px-0387Turtwig.png</t>
@@ -4339,10 +4339,10 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/b/b0/0411Bastiodon.png/70px-0411Bastiodon.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/4/42/0412Burmy-Trash.png/70px-0412Burmy-Trash.png</t>
-  </si>
-  <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/2/25/0413Wormadam-Trash.png/70px-0413Wormadam-Trash.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/e/e8/0412Burmy-Plant.png/70px-0412Burmy-Plant.png</t>
+  </si>
+  <si>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/e/ee/0413Wormadam-Plant.png/70px-0413Wormadam-Plant.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/2/22/0414Mothim.png/70px-0414Mothim.png</t>
@@ -4366,13 +4366,13 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/b/bc/0420Cherubi.png/70px-0420Cherubi.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/9/90/0421Cherrim-Sunshine.png/70px-0421Cherrim-Sunshine.png</t>
-  </si>
-  <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/d/db/0422Shellos-East.png/70px-0422Shellos-East.png</t>
-  </si>
-  <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/5/57/0423Gastrodon-East.png/70px-0423Gastrodon-East.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/2/21/0421Cherrim.png/70px-0421Cherrim.png</t>
+  </si>
+  <si>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/6/65/0422Shellos-West.png/70px-0422Shellos-West.png</t>
+  </si>
+  <si>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/c/c0/0423Gastrodon-West.png/70px-0423Gastrodon-West.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/9/9d/0424Ambipom.png/70px-0424Ambipom.png</t>
@@ -4540,7 +4540,7 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/5/59/0478Froslass.png/70px-0478Froslass.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/6/6d/0479Rotom-Mow.png/70px-0479Rotom-Mow.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/3/37/0479Rotom.png/70px-0479Rotom.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/1/18/0480Uxie.png/70px-0480Uxie.png</t>
@@ -4552,10 +4552,10 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/a/ac/0482Azelf.png/70px-0482Azelf.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/9/92/0483Dialga-Origin.png/70px-0483Dialga-Origin.png</t>
-  </si>
-  <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/1/12/0484Palkia-Origin.png/70px-0484Palkia-Origin.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/4/43/0483Dialga.png/70px-0483Dialga.png</t>
+  </si>
+  <si>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/b/b7/0484Palkia.png/70px-0484Palkia.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/6/60/0485Heatran.png/70px-0485Heatran.png</t>
@@ -4564,7 +4564,7 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/e/e3/0486Regigigas.png/70px-0486Regigigas.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/6/61/0487Giratina-Origin.png/70px-0487Giratina-Origin.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/8/81/0487Giratina.png/70px-0487Giratina.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/9/97/0488Cresselia.png/70px-0488Cresselia.png</t>
@@ -4579,7 +4579,7 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/8/88/0491Darkrai.png/70px-0491Darkrai.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/0/05/0492Shaymin-Sky.png/70px-0492Shaymin-Sky.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/0/09/0492Shaymin.png/70px-0492Shaymin.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/9/9e/0493Arceus.png/70px-0493Arceus.png</t>
@@ -4753,7 +4753,7 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/c/c1/0549Lilligant.png/70px-0549Lilligant.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/3/34/0550Basculin-White.png/70px-0550Basculin-White.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/4/41/0550Basculin-Red.png/70px-0550Basculin-Red.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/c/cb/0551Sandile.png/70px-0551Sandile.png</t>
@@ -4768,7 +4768,7 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/9/95/0554Darumaka.png/70px-0554Darumaka.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/8/88/0555Darmanitan-Zen.png/70px-0555Darmanitan-Zen.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/a/a3/0555Darmanitan.png/70px-0555Darmanitan.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/1/16/0556Maractus.png/70px-0556Maractus.png</t>
@@ -4858,10 +4858,10 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/b/b0/0584Vanilluxe.png/70px-0584Vanilluxe.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/2/20/0585Deerling-Winter.png/70px-0585Deerling-Winter.png</t>
-  </si>
-  <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/7/79/0586Sawsbuck-Winter.png/70px-0586Sawsbuck-Winter.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/c/c9/0585Deerling.png/70px-0585Deerling.png</t>
+  </si>
+  <si>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/b/ba/0586Sawsbuck.png/70px-0586Sawsbuck.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/9/96/0587Emolga.png/70px-0587Emolga.png</t>
@@ -5026,10 +5026,10 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/b/bf/0640Virizion.png/70px-0640Virizion.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/5/53/0641Tornadus-Therian.png/70px-0641Tornadus-Therian.png</t>
-  </si>
-  <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/3/3e/0642Thundurus-Therian.png/70px-0642Thundurus-Therian.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/1/12/0641Tornadus.png/70px-0641Tornadus.png</t>
+  </si>
+  <si>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/5/51/0642Thundurus.png/70px-0642Thundurus.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/5/56/0643Reshiram.png/70px-0643Reshiram.png</t>
@@ -5038,19 +5038,19 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/7/72/0644Zekrom.png/70px-0644Zekrom.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/4/44/0645Landorus-Therian.png/70px-0645Landorus-Therian.png</t>
-  </si>
-  <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/e/e8/0646Kyurem-Black.png/70px-0646Kyurem-Black.png</t>
-  </si>
-  <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/c/cf/0647Keldeo-Resolute.png/70px-0647Keldeo-Resolute.png</t>
-  </si>
-  <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/f/f9/0648Meloetta-Pirouette.png/70px-0648Meloetta-Pirouette.png</t>
-  </si>
-  <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/3/38/HOME0649W.png/70px-HOME0649W.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/d/da/0645Landorus.png/70px-0645Landorus.png</t>
+  </si>
+  <si>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/8/86/0646Kyurem.png/70px-0646Kyurem.png</t>
+  </si>
+  <si>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/9/92/0647Keldeo.png/70px-0647Keldeo.png</t>
+  </si>
+  <si>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/0/0b/0648Meloetta.png/70px-0648Meloetta.png</t>
+  </si>
+  <si>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/e/e3/0649Genesect.png/70px-0649Genesect.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/b/b0/0650Chespin.png/70px-0650Chespin.png</t>
@@ -5110,13 +5110,13 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/8/8a/0668Pyroar.png/70px-0668Pyroar.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/b/bf/HOME0669W.png/70px-HOME0669W.png</t>
-  </si>
-  <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/8/83/HOME0670W.png/70px-HOME0670W.png</t>
-  </si>
-  <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/d/d7/HOME0671W.png/70px-HOME0671W.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/5/5d/0669Flab%C3%A9b%C3%A9.png/70px-0669Flab%C3%A9b%C3%A9.png</t>
+  </si>
+  <si>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/8/8f/0670Floette.png/70px-0670Floette.png</t>
+  </si>
+  <si>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/0/0c/0671Florges.png/70px-0671Florges.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/e/e8/0672Skiddo.png/70px-0672Skiddo.png</t>
@@ -5137,7 +5137,7 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/1/1e/0677Espurr.png/70px-0677Espurr.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/1/1f/0678Meowstic-Female.png/70px-0678Meowstic-Female.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/6/6d/0678Meowstic-Male.png/70px-0678Meowstic-Male.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/4/48/0679Honedge.png/70px-0679Honedge.png</t>
@@ -5146,7 +5146,7 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/d/de/0680Doublade.png/70px-0680Doublade.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/9/99/0681Aegislash-Blade.png/70px-0681Aegislash-Blade.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/5/5a/0681Aegislash-Shield.png/70px-0681Aegislash-Shield.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/5/58/0682Spritzee.png/70px-0682Spritzee.png</t>
@@ -5251,19 +5251,19 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/7/7f/0715Noivern.png/70px-0715Noivern.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/1/17/0716Xerneas.png/70px-0716Xerneas.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/4/44/HOME0716N.png/70px-HOME0716N.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/1/1d/0717Yveltal.png/70px-0717Yveltal.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/f/fb/0718Zygarde-Complete.png/70px-0718Zygarde-Complete.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/9/92/0718Zygarde.png/70px-0718Zygarde.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/3/37/0719Diancie.png/70px-0719Diancie.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/a/a3/0720Hoopa-Unbound.png/70px-0720Hoopa-Unbound.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/7/71/0720Hoopa.png/70px-0720Hoopa.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/1/13/0721Volcanion.png/70px-0721Volcanion.png</t>
@@ -5326,7 +5326,7 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/2/29/0740Crabominable.png/70px-0740Crabominable.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/8/8d/0741Oricorio-Sensu.png/70px-0741Oricorio-Sensu.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/2/21/0741Oricorio.png/70px-0741Oricorio.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/f/f7/0742Cutiefly.png/70px-0742Cutiefly.png</t>
@@ -5338,10 +5338,10 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/6/6b/0744Rockruff.png/70px-0744Rockruff.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/7/7b/0745Lycanroc-Dusk.png/70px-0745Lycanroc-Dusk.png</t>
-  </si>
-  <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/a/a1/0746Wishiwashi-School.png/70px-0746Wishiwashi-School.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/b/b8/0745Lycanroc.png/70px-0745Lycanroc.png</t>
+  </si>
+  <si>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/c/c4/0746Wishiwashi.png/70px-0746Wishiwashi.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/6/63/0747Mareanie.png/70px-0747Mareanie.png</t>
@@ -5425,7 +5425,7 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/0/0d/0773Silvally.png/70px-0773Silvally.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/8/84/0774Minior-Core.png/70px-0774Minior-Core.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/4/4b/0774Minior.png/70px-0774Minior.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/f/f1/0775Komala.png/70px-0775Komala.png</t>
@@ -5437,7 +5437,7 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/8/8b/0777Togedemaru.png/70px-0777Togedemaru.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/4/4d/HOME0778B.png/70px-HOME0778B.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/4/41/0778Mimikyu.png/70px-0778Mimikyu.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/a/ac/0779Bruxish.png/70px-0779Bruxish.png</t>
@@ -5503,7 +5503,7 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/1/10/0799Guzzlord.png/70px-0799Guzzlord.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/6/67/0800Necrozma-Dawn_Wings.png/70px-0800Necrozma-Dawn_Wings.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/0/00/0800Necrozma.png/70px-0800Necrozma.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/c/cb/0801Magearna.png/70px-0801Magearna.png</t>
@@ -5638,7 +5638,7 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/b/b9/0844Sandaconda.png/70px-0844Sandaconda.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/7/78/0845Cramorant-Gorging.png/70px-0845Cramorant-Gorging.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/0/0d/0845Cramorant.png/70px-0845Cramorant.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/1/1f/0846Arrokuda.png/70px-0846Arrokuda.png</t>
@@ -5650,7 +5650,7 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/f/fa/0848Toxel.png/70px-0848Toxel.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/0/0f/0849Toxtricity-Low_Key.png/70px-0849Toxtricity-Low_Key.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/0/00/0849Toxtricity-Amped.png/70px-0849Toxtricity-Amped.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/9/9b/0850Sizzlipede.png/70px-0850Sizzlipede.png</t>
@@ -5728,13 +5728,13 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/f/ff/0874Stonjourner.png/70px-0874Stonjourner.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/f/fc/0875Eiscue-Noice.png/70px-0875Eiscue-Noice.png</t>
-  </si>
-  <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/4/4d/0876Indeedee-Female.png/70px-0876Indeedee-Female.png</t>
-  </si>
-  <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/2/28/0877Morpeko-Hangry.png/70px-0877Morpeko-Hangry.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/6/6d/0875Eiscue.png/70px-0875Eiscue.png</t>
+  </si>
+  <si>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/5/59/0876Indeedee-Male.png/70px-0876Indeedee-Male.png</t>
+  </si>
+  <si>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/e/ef/0877Morpeko-Full.png/70px-0877Morpeko-Full.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/9/9a/0878Cufant.png/70px-0878Cufant.png</t>
@@ -5767,10 +5767,10 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/e/e8/0887Dragapult.png/70px-0887Dragapult.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/9/98/0888Zacian.png/70px-0888Zacian.png</t>
-  </si>
-  <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/4/41/0889Zamazenta.png/70px-0889Zamazenta.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/3/32/0888Zacian-Hero.png/70px-0888Zacian-Hero.png</t>
+  </si>
+  <si>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/f/fc/0889Zamazenta-Hero.png/70px-0889Zamazenta-Hero.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/0/0e/0890Eternatus.png/70px-0890Eternatus.png</t>
@@ -5779,7 +5779,7 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/1/14/0891Kubfu.png/70px-0891Kubfu.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/4/4a/0892Urshifu-Rapid_Strike.png/70px-0892Urshifu-Rapid_Strike.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/5/57/0892Urshifu-Single_Strike.png/70px-0892Urshifu-Single_Strike.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/b/bf/0893Zarude.png/70px-0893Zarude.png</t>
@@ -5797,7 +5797,7 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/e/ef/0897Spectrier.png/70px-0897Spectrier.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/9/9b/0898Calyrex-Shadow_Rider.png/70px-0898Calyrex-Shadow_Rider.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/8/80/0898Calyrex.png/70px-0898Calyrex.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/9/97/0899Wyrdeer.png/70px-0899Wyrdeer.png</t>
@@ -5806,10 +5806,10 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/8/8f/0900Kleavor.png/70px-0900Kleavor.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/8/85/0901Ursaluna-Bloodmoon.png/70px-0901Ursaluna-Bloodmoon.png</t>
-  </si>
-  <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/7/73/0902Basculegion-Female.png/70px-0902Basculegion-Female.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/7/7c/0901Ursaluna.png/70px-0901Ursaluna.png</t>
+  </si>
+  <si>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/e/e1/0902Basculegion-Male.png/70px-0902Basculegion-Male.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/a/a3/0903Sneasler.png/70px-0903Sneasler.png</t>
@@ -5818,7 +5818,7 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/0/02/0904Overqwil.png/70px-0904Overqwil.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/4/43/0905Enamorus-Therian.png/70px-0905Enamorus-Therian.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/5/54/0905Enamorus.png/70px-0905Enamorus.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/e/e2/0906Sprigatito.png/70px-0906Sprigatito.png</t>
@@ -5851,7 +5851,7 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/7/75/0915Lechonk.png/70px-0915Lechonk.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/d/d8/0916Oinkologne-Female.png/70px-0916Oinkologne-Female.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/3/32/0916Oinkologne-Male.png/70px-0916Oinkologne-Male.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/e/e4/0917Tarountula.png/70px-0917Tarountula.png</t>
@@ -5878,7 +5878,7 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/a/ab/0924Tandemaus.png/70px-0924Tandemaus.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/f/f4/0925Maushold.png/70px-0925Maushold.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/a/ab/0925Maushold-Three.png/70px-0925Maushold-Three.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/8/82/0926Fidough.png/70px-0926Fidough.png</t>
@@ -5896,7 +5896,7 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/a/ab/0930Arboliva.png/70px-0930Arboliva.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/a/a8/0931Squawkabilly-White.png/70px-0931Squawkabilly-White.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/d/d6/0931Squawkabilly.png/70px-0931Squawkabilly.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/f/f5/0932Nacli.png/70px-0932Nacli.png</t>
@@ -5995,7 +5995,7 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/a/a5/0963Finizen.png/70px-0963Finizen.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/4/43/0964Palafin-Hero.png/70px-0964Palafin-Hero.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/7/7a/0964Palafin.png/70px-0964Palafin.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/d/d1/0965Varoom.png/70px-0965Varoom.png</t>
@@ -6037,7 +6037,7 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/b/b8/0977Dondozo.png/70px-0977Dondozo.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/0/06/0978Tatsugiri-Stretchy.png/70px-0978Tatsugiri-Stretchy.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/3/34/0978Tatsugiri.png/70px-0978Tatsugiri.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/a/a7/0979Annihilape.png/70px-0979Annihilape.png</t>
@@ -6049,7 +6049,7 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/0/03/0981Farigiraf.png/70px-0981Farigiraf.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/a/ab/0982Dudunsparce-Three.png/70px-0982Dudunsparce-Three.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/6/65/0982Dudunsparce.png/70px-0982Dudunsparce.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/7/7f/0983Kingambit.png/70px-0983Kingambit.png</t>
@@ -6100,7 +6100,7 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/7/70/0998Baxcalibur.png/70px-0998Baxcalibur.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/4/40/0999Gimmighoul-Roaming.png/70px-0999Gimmighoul-Roaming.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/6/6f/0999Gimmighoul.png/70px-0999Gimmighoul.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/2/2d/1000Gholdengo.png/70px-1000Gholdengo.png</t>
@@ -6154,7 +6154,7 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/c/cb/1016Fezandipiti.png/70px-1016Fezandipiti.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/4/4d/1017Ogerpon-Cornerstone_Mask.png/70px-1017Ogerpon-Cornerstone_Mask.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/a/a5/1017Ogerpon.png/70px-1017Ogerpon.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/c/c4/1018Archaludon.png/70px-1018Archaludon.png</t>
@@ -6175,7 +6175,7 @@
     <t>https://archives.bulbagarden.net/media/upload/thumb/3/3a/1023Iron_Crown.png/70px-1023Iron_Crown.png</t>
   </si>
   <si>
-    <t>https://archives.bulbagarden.net/media/upload/thumb/e/ed/1024Terapagos-Terastal.png/70px-1024Terapagos-Terastal.png</t>
+    <t>https://archives.bulbagarden.net/media/upload/thumb/d/d1/1024Terapagos.png/70px-1024Terapagos.png</t>
   </si>
   <si>
     <t>https://archives.bulbagarden.net/media/upload/thumb/5/5a/1025Pecharunt.png/70px-1025Pecharunt.png</t>

</xml_diff>